<commit_message>
Grafik Terbaru dari Google Scholar
</commit_message>
<xml_diff>
--- a/Grafik Paper tahunan.xlsx
+++ b/Grafik Paper tahunan.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\College\6th Semester\Metodologi Penelitian\Pertemuan 13 (01-06-2021)\Metpen_BCI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E45932-0319-448C-B383-29C107F6CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-6675" yWindow="1830" windowWidth="21600" windowHeight="11835" xr2:uid="{82CDA055-CE4B-4FAE-A40C-0254FAC6B7B2}"/>
+    <workbookView xWindow="-6675" yWindow="1830" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,9 +42,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -102,7 +96,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -112,10 +106,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -142,7 +136,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -162,30 +174,9 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -208,7 +199,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -227,7 +217,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -246,7 +235,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -271,7 +259,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -290,7 +277,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -309,7 +295,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -353,6 +339,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -361,26 +348,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -460,7 +427,7 @@
             <c:numRef>
               <c:f>All!$C$2:$C$12</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>433</c:v>
@@ -499,7 +466,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0886-470E-87F0-0342BB645E70}"/>
             </c:ext>
@@ -579,7 +546,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)">
+                <c:pt idx="0" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -616,7 +583,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0886-470E-87F0-0342BB645E70}"/>
             </c:ext>
@@ -694,46 +661,46 @@
             <c:numRef>
               <c:f>All!$E$2:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3190</c:v>
+                  <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3550</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4590</c:v>
+                  <c:v>1040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4800</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5350</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5600</c:v>
+                  <c:v>1110</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6430</c:v>
+                  <c:v>1210</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7270</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7980</c:v>
+                  <c:v>1150</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7980</c:v>
+                  <c:v>777</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3420</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0886-470E-87F0-0342BB645E70}"/>
             </c:ext>
@@ -747,12 +714,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2022380688"/>
-        <c:axId val="2022381936"/>
+        <c:axId val="194561152"/>
+        <c:axId val="194562688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2022380688"/>
+        <c:axId val="194561152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,7 +763,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2022381936"/>
+        <c:crossAx val="194562688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -803,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2022381936"/>
+        <c:axId val="194562688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +791,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -854,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2022380688"/>
+        <c:crossAx val="194561152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -868,6 +836,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1510,7 +1479,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EEE0B07-9EBD-4BEB-A033-7F0423FB3B53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5EEE0B07-9EBD-4BEB-A033-7F0423FB3B53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1532,14 +1501,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12BFBE2E-B195-498E-944E-E8EE2EC2E235}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Comma [0]">
-  <autoFilter ref="A1:E12" xr:uid="{12BFBE2E-B195-498E-944E-E8EE2EC2E235}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E13" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Comma [0]">
+  <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C10F9C85-22BB-4381-8BFB-423464498607}" name="No" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A755C43D-BF76-4075-ACD3-AABFD2F2C50E}" name="Tahun" dataDxfId="8" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{AD344DF3-D0B9-43B6-AAC9-BFAC2E2F046B}" name="IEEE" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Comma [0]"/>
-    <tableColumn id="4" xr3:uid="{24B359CA-B066-4512-8E43-508FFABC100D}" name="Science Direct" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
-    <tableColumn id="5" xr3:uid="{4CDC3ADA-8992-4258-8A41-D964CADDF7F0}" name="Google Scholar" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="1" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" name="No" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Tahun" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="IEEE" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Comma [0]"/>
+    <tableColumn id="4" name="Science Direct" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="1" dataCellStyle="Comma [0]"/>
+    <tableColumn id="5" name="Google Scholar" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1588,7 +1557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1640,7 +1609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1834,18 +1803,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65164F8E-615F-497C-9607-6B576C190DA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>3190</v>
+        <v>865</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,7 +1872,7 @@
         <v>1736</v>
       </c>
       <c r="E3" s="3">
-        <v>3550</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,7 +1889,7 @@
         <v>1742</v>
       </c>
       <c r="E4" s="3">
-        <v>4590</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,7 +1906,7 @@
         <v>1942</v>
       </c>
       <c r="E5" s="3">
-        <v>4800</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1954,7 +1923,7 @@
         <v>2076</v>
       </c>
       <c r="E6" s="3">
-        <v>5350</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1971,7 +1940,7 @@
         <v>2000</v>
       </c>
       <c r="E7" s="3">
-        <v>5600</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,7 +1957,7 @@
         <v>2109</v>
       </c>
       <c r="E8" s="3">
-        <v>6430</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,7 +1974,7 @@
         <v>2302</v>
       </c>
       <c r="E9" s="3">
-        <v>7270</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2022,7 +1991,7 @@
         <v>2424</v>
       </c>
       <c r="E10" s="3">
-        <v>7980</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2039,7 +2008,7 @@
         <v>2918</v>
       </c>
       <c r="E11" s="3">
-        <v>7980</v>
+        <v>777</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2056,7 +2025,7 @@
         <v>2173</v>
       </c>
       <c r="E12" s="3">
-        <v>3420</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2043,7 @@
       </c>
       <c r="E13" s="4">
         <f>SUBTOTAL(109,Table1[Google Scholar])</f>
-        <v>60160</v>
+        <v>10674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>